<commit_message>
bugfix: For table width adjustment.
</commit_message>
<xml_diff>
--- a/docs/Template.xlsx
+++ b/docs/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pearl\Downloads\WebApp_v1.2\WebApp\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pearl\Documents\DevProjects\jlpt-reviewer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17715" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17715" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="N4ごい➀" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Kanji_N4L12-15" sheetId="4" r:id="rId5"/>
     <sheet name="Kanji_N4L16-18" sheetId="2" r:id="rId6"/>
     <sheet name="Kanji_N4L19-20" sheetId="3" r:id="rId7"/>
+    <sheet name="漢字N3W1D1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="1489">
   <si>
     <t>とどけます</t>
   </si>
@@ -5602,6 +5603,252 @@
   </si>
   <si>
     <t>cure; fix (intransitive)</t>
+  </si>
+  <si>
+    <t>駐</t>
+  </si>
+  <si>
+    <t>駐車</t>
+  </si>
+  <si>
+    <t>駐車場</t>
+  </si>
+  <si>
+    <t>parking lot</t>
+  </si>
+  <si>
+    <t>無</t>
+  </si>
+  <si>
+    <t>stop-over;reside in;resident</t>
+  </si>
+  <si>
+    <t>park;parking</t>
+  </si>
+  <si>
+    <t>does not exist;do not have;gone</t>
+  </si>
+  <si>
+    <t>無い</t>
+  </si>
+  <si>
+    <t>無休</t>
+  </si>
+  <si>
+    <t>work without a holiday;work without a holiday</t>
+  </si>
+  <si>
+    <t>not existing; none</t>
+  </si>
+  <si>
+    <t>unreasonable;impossible</t>
+  </si>
+  <si>
+    <t>無料</t>
+  </si>
+  <si>
+    <t>free;free of charge</t>
+  </si>
+  <si>
+    <t>満車</t>
+  </si>
+  <si>
+    <t>being full;full</t>
+  </si>
+  <si>
+    <t>満</t>
+  </si>
+  <si>
+    <t>ちゅう;cyuu;chuu</t>
+  </si>
+  <si>
+    <t>む;ない;mu;nai</t>
+  </si>
+  <si>
+    <t>むきゅう;mukyuu</t>
+  </si>
+  <si>
+    <t>むり;むりな;muri;murina</t>
+  </si>
+  <si>
+    <t>無理(な)</t>
+  </si>
+  <si>
+    <t>むりょう;muryou</t>
+  </si>
+  <si>
+    <t>ない;nai</t>
+  </si>
+  <si>
+    <t>まん;man</t>
+  </si>
+  <si>
+    <t>まんしゃ;mansya;mansha</t>
+  </si>
+  <si>
+    <t>ちゅうしゃ;cyuusya;chuusya;cyuusha;chuusha</t>
+  </si>
+  <si>
+    <t>ちゅうしゃじょう;cyuusyajyou;chuusyajyou;cyuushajyou;chuushajyou</t>
+  </si>
+  <si>
+    <t>full of cars;full (of cars);full(of cars)</t>
+  </si>
+  <si>
+    <t>不満(な)</t>
+  </si>
+  <si>
+    <t>ふまん;ふまんな;fuman;fumanna</t>
+  </si>
+  <si>
+    <t>dissatisfaction;dissatisfied</t>
+  </si>
+  <si>
+    <t>満員</t>
+  </si>
+  <si>
+    <t>まんいん;manin;manin</t>
+  </si>
+  <si>
+    <t>full of people;full (of people);full(of people)</t>
+  </si>
+  <si>
+    <t>向</t>
+  </si>
+  <si>
+    <t>こう;むこう;むかう;むき;kou;mukou;mukau;muki</t>
+  </si>
+  <si>
+    <t>facing;toward;beyond</t>
+  </si>
+  <si>
+    <t>方向</t>
+  </si>
+  <si>
+    <t>ほうこう;houkou</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>向かう</t>
+  </si>
+  <si>
+    <t>向かう;mukau</t>
+  </si>
+  <si>
+    <t>go forward</t>
+  </si>
+  <si>
+    <t>向こう</t>
+  </si>
+  <si>
+    <t>むこう;mukou</t>
+  </si>
+  <si>
+    <t>over there;beyond</t>
+  </si>
+  <si>
+    <t>○○向き</t>
+  </si>
+  <si>
+    <t>むき;muki</t>
+  </si>
+  <si>
+    <t>suitable for</t>
+  </si>
+  <si>
+    <t>禁</t>
+  </si>
+  <si>
+    <t>ban;prohibition</t>
+  </si>
+  <si>
+    <t>きん;kin</t>
+  </si>
+  <si>
+    <t>禁止</t>
+  </si>
+  <si>
+    <t>きんし;kinshi</t>
+  </si>
+  <si>
+    <t>関</t>
+  </si>
+  <si>
+    <t>かん;せき;kan;seki;</t>
+  </si>
+  <si>
+    <t>barrier;gate;connection;related</t>
+  </si>
+  <si>
+    <t>関心</t>
+  </si>
+  <si>
+    <t>かんしん;kanshin</t>
+  </si>
+  <si>
+    <t>関する</t>
+  </si>
+  <si>
+    <t>かんする;kansuru</t>
+  </si>
+  <si>
+    <t>related</t>
+  </si>
+  <si>
+    <t>関係</t>
+  </si>
+  <si>
+    <t>係</t>
+  </si>
+  <si>
+    <t>かんけい;kankei</t>
+  </si>
+  <si>
+    <t>relation;connection</t>
+  </si>
+  <si>
+    <t>かかり;kakari</t>
+  </si>
+  <si>
+    <t>person in charge</t>
+  </si>
+  <si>
+    <t>断</t>
+  </si>
+  <si>
+    <t>だん;dan</t>
+  </si>
+  <si>
+    <t>decision;judgement;resolution</t>
+  </si>
+  <si>
+    <t>無断</t>
+  </si>
+  <si>
+    <t>むだん;mudan</t>
+  </si>
+  <si>
+    <t>without permission</t>
+  </si>
+  <si>
+    <t>断る</t>
+  </si>
+  <si>
+    <t>ことわる;kotowaru</t>
+  </si>
+  <si>
+    <t>refuse</t>
+  </si>
+  <si>
+    <t>断水</t>
+  </si>
+  <si>
+    <t>だんすい;dansui</t>
+  </si>
+  <si>
+    <t>suspension of water supply</t>
   </si>
 </sst>
 </file>
@@ -5731,57 +5978,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7258,7 +7455,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9240,7 +9437,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9309,7 +9506,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f t="shared" ref="F1:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <f t="shared" ref="F2:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
         <v>映す,うつす,to reflect,~,~</v>
       </c>
       <c r="G2" s="3" t="str">
@@ -11819,10 +12016,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11891,7 +12088,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f t="shared" ref="F1:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <f t="shared" ref="F2:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
         <v>体,からだ,body,~,~</v>
       </c>
       <c r="G2" s="3" t="str">
@@ -13237,10 +13434,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13309,11 +13506,11 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f t="shared" ref="F1:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <f t="shared" ref="F2:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
         <v>家,いえ,house,~,~</v>
       </c>
       <c r="G2" s="3" t="str">
-        <f>CONCATENATE(A2,",",C2,",",B2,",",D2,",",E2)</f>
+        <f t="shared" ref="G2:G33" si="1">CONCATENATE(A2,",",C2,",",B2,",",D2,",",E2)</f>
         <v>家,house,いえ,~,~</v>
       </c>
     </row>
@@ -13338,7 +13535,7 @@
         <v>画家,がか,painter,~,~</v>
       </c>
       <c r="G3" s="3" t="str">
-        <f>CONCATENATE(A3,",",C3,",",B3,",",D3,",",E3)</f>
+        <f t="shared" si="1"/>
         <v>画家,painter,がか,~,~</v>
       </c>
     </row>
@@ -13363,7 +13560,7 @@
         <v>家内,かない,wife,~,~</v>
       </c>
       <c r="G4" s="3" t="str">
-        <f>CONCATENATE(A4,",",C4,",",B4,",",D4,",",E4)</f>
+        <f t="shared" si="1"/>
         <v>家内,wife,かない,~,~</v>
       </c>
     </row>
@@ -13388,7 +13585,7 @@
         <v>家族,かぞく,family,~,~</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>CONCATENATE(A5,",",C5,",",B5,",",D5,",",E5)</f>
+        <f t="shared" si="1"/>
         <v>家族,family,かぞく,~,~</v>
       </c>
     </row>
@@ -13413,7 +13610,7 @@
         <v>私,わたし,I,~,~</v>
       </c>
       <c r="G6" s="3" t="str">
-        <f>CONCATENATE(A6,",",C6,",",B6,",",D6,",",E6)</f>
+        <f t="shared" si="1"/>
         <v>私,I,わたし,~,~</v>
       </c>
     </row>
@@ -13438,7 +13635,7 @@
         <v>自分,じぶん,oneself,~,~</v>
       </c>
       <c r="G7" s="3" t="str">
-        <f>CONCATENATE(A7,",",C7,",",B7,",",D7,",",E7)</f>
+        <f t="shared" si="1"/>
         <v>自分,oneself,じぶん,~,~</v>
       </c>
     </row>
@@ -13463,7 +13660,7 @@
         <v>自動ドア,じどうドア,automatic door,~,~</v>
       </c>
       <c r="G8" s="3" t="str">
-        <f>CONCATENATE(A8,",",C8,",",B8,",",D8,",",E8)</f>
+        <f t="shared" si="1"/>
         <v>自動ドア,automatic door,じどうドア,~,~</v>
       </c>
     </row>
@@ -13488,7 +13685,7 @@
         <v>親,おや,parent,~,~</v>
       </c>
       <c r="G9" s="3" t="str">
-        <f>CONCATENATE(A9,",",C9,",",B9,",",D9,",",E9)</f>
+        <f t="shared" si="1"/>
         <v>親,parent,おや,~,~</v>
       </c>
     </row>
@@ -13513,7 +13710,7 @@
         <v>母親,ははおや,mother,~,~</v>
       </c>
       <c r="G10" s="3" t="str">
-        <f>CONCATENATE(A10,",",C10,",",B10,",",D10,",",E10)</f>
+        <f t="shared" si="1"/>
         <v>母親,mother,ははおや,~,~</v>
       </c>
     </row>
@@ -13538,7 +13735,7 @@
         <v>親切な,しんせつな,kind,~,~</v>
       </c>
       <c r="G11" s="3" t="str">
-        <f>CONCATENATE(A11,",",C11,",",B11,",",D11,",",E11)</f>
+        <f t="shared" si="1"/>
         <v>親切な,kind,しんせつな,~,~</v>
       </c>
     </row>
@@ -13563,7 +13760,7 @@
         <v>両親,りょうしん,parents,~,~</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f>CONCATENATE(A12,",",C12,",",B12,",",D12,",",E12)</f>
+        <f t="shared" si="1"/>
         <v>両親,parents,りょうしん,~,~</v>
       </c>
     </row>
@@ -13588,7 +13785,7 @@
         <v>両方,りょうほう,both,~,~</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f>CONCATENATE(A13,",",C13,",",B13,",",D13,",",E13)</f>
+        <f t="shared" si="1"/>
         <v>両方,both,りょうほう,~,~</v>
       </c>
     </row>
@@ -13613,7 +13810,7 @@
         <v>両手,りょうて,both hands,~,~</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>CONCATENATE(A14,",",C14,",",B14,",",D14,",",E14)</f>
+        <f t="shared" si="1"/>
         <v>両手,both hands,りょうて,~,~</v>
       </c>
     </row>
@@ -13638,7 +13835,7 @@
         <v>兄,あに,one’s elder brother,~,~</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f>CONCATENATE(A15,",",C15,",",B15,",",D15,",",E15)</f>
+        <f t="shared" si="1"/>
         <v>兄,one’s elder brother,あに,~,~</v>
       </c>
     </row>
@@ -13663,7 +13860,7 @@
         <v>お兄さん,おにいさん,elder brother,~,~</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f>CONCATENATE(A16,",",C16,",",B16,",",D16,",",E16)</f>
+        <f t="shared" si="1"/>
         <v>お兄さん,elder brother,おにいさん,~,~</v>
       </c>
     </row>
@@ -13688,7 +13885,7 @@
         <v>弟,おとうと,one’s younger brother,~,~</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f>CONCATENATE(A17,",",C17,",",B17,",",D17,",",E17)</f>
+        <f t="shared" si="1"/>
         <v>弟,one’s younger brother,おとうと,~,~</v>
       </c>
     </row>
@@ -13713,7 +13910,7 @@
         <v>兄弟,きょうだい,brothers / siblings,~,~</v>
       </c>
       <c r="G18" s="3" t="str">
-        <f>CONCATENATE(A18,",",C18,",",B18,",",D18,",",E18)</f>
+        <f t="shared" si="1"/>
         <v>兄弟,brothers / siblings,きょうだい,~,~</v>
       </c>
     </row>
@@ -13738,7 +13935,7 @@
         <v>姉,あね,one’s elder sister,~,~</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f>CONCATENATE(A19,",",C19,",",B19,",",D19,",",E19)</f>
+        <f t="shared" si="1"/>
         <v>姉,one’s elder sister,あね,~,~</v>
       </c>
     </row>
@@ -13763,7 +13960,7 @@
         <v>お姉さん,おねえさん,elder sister,~,~</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f>CONCATENATE(A20,",",C20,",",B20,",",D20,",",E20)</f>
+        <f t="shared" si="1"/>
         <v>お姉さん,elder sister,おねえさん,~,~</v>
       </c>
     </row>
@@ -13788,7 +13985,7 @@
         <v>妹,いもうと,one’s younger sister,~,~</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f>CONCATENATE(A21,",",C21,",",B21,",",D21,",",E21)</f>
+        <f t="shared" si="1"/>
         <v>妹,one’s younger sister,いもうと,~,~</v>
       </c>
     </row>
@@ -13813,7 +14010,7 @@
         <v>姉妹,しまい,sisters,~,~</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f>CONCATENATE(A22,",",C22,",",B22,",",D22,",",E22)</f>
+        <f t="shared" si="1"/>
         <v>姉妹,sisters,しまい,~,~</v>
       </c>
     </row>
@@ -13838,7 +14035,7 @@
         <v>生活,せいかつ,living,~,~</v>
       </c>
       <c r="G23" s="3" t="str">
-        <f>CONCATENATE(A23,",",C23,",",B23,",",D23,",",E23)</f>
+        <f t="shared" si="1"/>
         <v>生活,living,せいかつ,~,~</v>
       </c>
     </row>
@@ -13863,7 +14060,7 @@
         <v>回す,まわす,to turn,~,~</v>
       </c>
       <c r="G24" s="3" t="str">
-        <f>CONCATENATE(A24,",",C24,",",B24,",",D24,",",E24)</f>
+        <f t="shared" si="1"/>
         <v>回す,to turn,まわす,~,~</v>
       </c>
     </row>
@@ -13888,7 +14085,7 @@
         <v>１回,いっかい,once,~,~</v>
       </c>
       <c r="G25" s="3" t="str">
-        <f>CONCATENATE(A25,",",C25,",",B25,",",D25,",",E25)</f>
+        <f t="shared" si="1"/>
         <v>１回,once,いっかい,~,~</v>
       </c>
     </row>
@@ -13913,7 +14110,7 @@
         <v>前回,ぜんかい,the last time,~,~</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>CONCATENATE(A26,",",C26,",",B26,",",D26,",",E26)</f>
+        <f t="shared" si="1"/>
         <v>前回,the last time,ぜんかい,~,~</v>
       </c>
     </row>
@@ -13938,7 +14135,7 @@
         <v>主人,しゅじん,husband,~,~</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f>CONCATENATE(A27,",",C27,",",B27,",",D27,",",E27)</f>
+        <f t="shared" si="1"/>
         <v>主人,husband,しゅじん,~,~</v>
       </c>
     </row>
@@ -13963,7 +14160,7 @@
         <v>色,いろ,color,~,~</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f>CONCATENATE(A28,",",C28,",",B28,",",D28,",",E28)</f>
+        <f t="shared" si="1"/>
         <v>色,color,いろ,~,~</v>
       </c>
     </row>
@@ -13988,7 +14185,7 @@
         <v>茶色,ちゃいろ,brown,~,~</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f>CONCATENATE(A29,",",C29,",",B29,",",D29,",",E29)</f>
+        <f t="shared" si="1"/>
         <v>茶色,brown,ちゃいろ,~,~</v>
       </c>
     </row>
@@ -14013,7 +14210,7 @@
         <v>形,かたち,shape,~,~</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f>CONCATENATE(A30,",",C30,",",B30,",",D30,",",E30)</f>
+        <f t="shared" si="1"/>
         <v>形,shape,かたち,~,~</v>
       </c>
     </row>
@@ -14038,7 +14235,7 @@
         <v>人形,にんぎょう,doll,~,~</v>
       </c>
       <c r="G31" s="3" t="str">
-        <f>CONCATENATE(A31,",",C31,",",B31,",",D31,",",E31)</f>
+        <f t="shared" si="1"/>
         <v>人形,doll,にんぎょう,~,~</v>
       </c>
     </row>
@@ -14063,7 +14260,7 @@
         <v>品物,しなもの,goods,~,~</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f>CONCATENATE(A32,",",C32,",",B32,",",D32,",",E32)</f>
+        <f t="shared" si="1"/>
         <v>品物,goods,しなもの,~,~</v>
       </c>
     </row>
@@ -14084,11 +14281,11 @@
         <v>7</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f t="shared" ref="F33:F64" si="1">CONCATENATE(A33,",",B33,",",C33,",",D33,",",E33)</f>
+        <f t="shared" ref="F33:F64" si="2">CONCATENATE(A33,",",B33,",",C33,",",D33,",",E33)</f>
         <v>食料品,しょくりょうひん,food,~,~</v>
       </c>
       <c r="G33" s="3" t="str">
-        <f>CONCATENATE(A33,",",C33,",",B33,",",D33,",",E33)</f>
+        <f t="shared" si="1"/>
         <v>食料品,food,しょくりょうひん,~,~</v>
       </c>
     </row>
@@ -14109,11 +14306,11 @@
         <v>7</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>国民,こくみん,citizens of the state,~,~</v>
       </c>
       <c r="G34" s="3" t="str">
-        <f>CONCATENATE(A34,",",C34,",",B34,",",D34,",",E34)</f>
+        <f t="shared" ref="G34:G65" si="3">CONCATENATE(A34,",",C34,",",B34,",",D34,",",E34)</f>
         <v>国民,citizens of the state,こくみん,~,~</v>
       </c>
     </row>
@@ -14134,11 +14331,11 @@
         <v>7</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>市民,しみん,citizen,~,~</v>
       </c>
       <c r="G35" s="3" t="str">
-        <f>CONCATENATE(A35,",",C35,",",B35,",",D35,",",E35)</f>
+        <f t="shared" si="3"/>
         <v>市民,citizen,しみん,~,~</v>
       </c>
     </row>
@@ -14159,11 +14356,11 @@
         <v>7</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>服,ふく,clothes,~,~</v>
       </c>
       <c r="G36" s="3" t="str">
-        <f>CONCATENATE(A36,",",C36,",",B36,",",D36,",",E36)</f>
+        <f t="shared" si="3"/>
         <v>服,clothes,ふく,~,~</v>
       </c>
     </row>
@@ -14184,11 +14381,11 @@
         <v>7</v>
       </c>
       <c r="F37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>洋服,ようふく,Western clothing,~,~</v>
       </c>
       <c r="G37" s="3" t="str">
-        <f>CONCATENATE(A37,",",C37,",",B37,",",D37,",",E37)</f>
+        <f t="shared" si="3"/>
         <v>洋服,Western clothing,ようふく,~,~</v>
       </c>
     </row>
@@ -14209,11 +14406,11 @@
         <v>7</v>
       </c>
       <c r="F38" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>犬,いぬ,dog,~,~</v>
       </c>
       <c r="G38" s="3" t="str">
-        <f>CONCATENATE(A38,",",C38,",",B38,",",D38,",",E38)</f>
+        <f t="shared" si="3"/>
         <v>犬,dog,いぬ,~,~</v>
       </c>
     </row>
@@ -14234,11 +14431,11 @@
         <v>7</v>
       </c>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>子犬,こいぬ,puppy,~,~</v>
       </c>
       <c r="G39" s="3" t="str">
-        <f>CONCATENATE(A39,",",C39,",",B39,",",D39,",",E39)</f>
+        <f t="shared" si="3"/>
         <v>子犬,puppy,こいぬ,~,~</v>
       </c>
     </row>
@@ -14259,11 +14456,11 @@
         <v>7</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>同じ,おなじ,same,~,~</v>
       </c>
       <c r="G40" s="3" t="str">
-        <f>CONCATENATE(A40,",",C40,",",B40,",",D40,",",E40)</f>
+        <f t="shared" si="3"/>
         <v>同じ,same,おなじ,~,~</v>
       </c>
     </row>
@@ -14284,11 +14481,11 @@
         <v>7</v>
       </c>
       <c r="F41" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>米,こめ,rice,~,~</v>
       </c>
       <c r="G41" s="3" t="str">
-        <f>CONCATENATE(A41,",",C41,",",B41,",",D41,",",E41)</f>
+        <f t="shared" si="3"/>
         <v>米,rice,こめ,~,~</v>
       </c>
     </row>
@@ -14309,11 +14506,11 @@
         <v>7</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>料金,りょうきん,fee; charge,~,~</v>
       </c>
       <c r="G42" s="3" t="str">
-        <f>CONCATENATE(A42,",",C42,",",B42,",",D42,",",E42)</f>
+        <f t="shared" si="3"/>
         <v>料金,fee; charge,りょうきん,~,~</v>
       </c>
     </row>
@@ -14334,11 +14531,11 @@
         <v>7</v>
       </c>
       <c r="F43" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>料理,りょうり,cooking,~,~</v>
       </c>
       <c r="G43" s="3" t="str">
-        <f>CONCATENATE(A43,",",C43,",",B43,",",D43,",",E43)</f>
+        <f t="shared" si="3"/>
         <v>料理,cooking,りょうり,~,~</v>
       </c>
     </row>
@@ -14359,11 +14556,11 @@
         <v>7</v>
       </c>
       <c r="F44" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>地理,ちり,geography,~,~</v>
       </c>
       <c r="G44" s="3" t="str">
-        <f>CONCATENATE(A44,",",C44,",",B44,",",D44,",",E44)</f>
+        <f t="shared" si="3"/>
         <v>地理,geography,ちり,~,~</v>
       </c>
     </row>
@@ -14384,11 +14581,11 @@
         <v>7</v>
       </c>
       <c r="F45" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>肉,にく,meat,~,~</v>
       </c>
       <c r="G45" s="3" t="str">
-        <f>CONCATENATE(A45,",",C45,",",B45,",",D45,",",E45)</f>
+        <f t="shared" si="3"/>
         <v>肉,meat,にく,~,~</v>
       </c>
     </row>
@@ -14409,11 +14606,11 @@
         <v>7</v>
       </c>
       <c r="F46" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>牛肉,ぎゅうにく,beef,~,~</v>
       </c>
       <c r="G46" s="3" t="str">
-        <f>CONCATENATE(A46,",",C46,",",B46,",",D46,",",E46)</f>
+        <f t="shared" si="3"/>
         <v>牛肉,beef,ぎゅうにく,~,~</v>
       </c>
     </row>
@@ -14434,11 +14631,11 @@
         <v>7</v>
       </c>
       <c r="F47" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>鳥,とり,bird,~,~</v>
       </c>
       <c r="G47" s="3" t="str">
-        <f>CONCATENATE(A47,",",C47,",",B47,",",D47,",",E47)</f>
+        <f t="shared" si="3"/>
         <v>鳥,bird,とり,~,~</v>
       </c>
     </row>
@@ -14459,11 +14656,11 @@
         <v>7</v>
       </c>
       <c r="F48" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>小鳥,ことり,little bird,~,~</v>
       </c>
       <c r="G48" s="3" t="str">
-        <f>CONCATENATE(A48,",",C48,",",B48,",",D48,",",E48)</f>
+        <f t="shared" si="3"/>
         <v>小鳥,little bird,ことり,~,~</v>
       </c>
     </row>
@@ -14484,11 +14681,11 @@
         <v>7</v>
       </c>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>鳥肉,とりにく,chicken,~,~</v>
       </c>
       <c r="G49" s="3" t="str">
-        <f>CONCATENATE(A49,",",C49,",",B49,",",D49,",",E49)</f>
+        <f t="shared" si="3"/>
         <v>鳥肉,chicken,とりにく,~,~</v>
       </c>
     </row>
@@ -14509,11 +14706,11 @@
         <v>7</v>
       </c>
       <c r="F50" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>野菜,やさい,vegetable,~,~</v>
       </c>
       <c r="G50" s="3" t="str">
-        <f>CONCATENATE(A50,",",C50,",",B50,",",D50,",",E50)</f>
+        <f t="shared" si="3"/>
         <v>野菜,vegetable,やさい,~,~</v>
       </c>
     </row>
@@ -14534,11 +14731,11 @@
         <v>7</v>
       </c>
       <c r="F51" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>お茶,おちゃ,tea,~,~</v>
       </c>
       <c r="G51" s="3" t="str">
-        <f>CONCATENATE(A51,",",C51,",",B51,",",D51,",",E51)</f>
+        <f t="shared" si="3"/>
         <v>お茶,tea,おちゃ,~,~</v>
       </c>
     </row>
@@ -14559,11 +14756,11 @@
         <v>7</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ご飯,ごはん,cooked rice; meal,~,~</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f>CONCATENATE(A52,",",C52,",",B52,",",D52,",",E52)</f>
+        <f t="shared" si="3"/>
         <v>ご飯,cooked rice; meal,ごはん,~,~</v>
       </c>
     </row>
@@ -14584,11 +14781,11 @@
         <v>7</v>
       </c>
       <c r="F53" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>夕飯,ゆうはん,supper,~,~</v>
       </c>
       <c r="G53" s="3" t="str">
-        <f>CONCATENATE(A53,",",C53,",",B53,",",D53,",",E53)</f>
+        <f t="shared" si="3"/>
         <v>夕飯,supper,ゆうはん,~,~</v>
       </c>
     </row>
@@ -14609,11 +14806,11 @@
         <v>7</v>
       </c>
       <c r="F54" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>晩ご飯,ばんごはん,dinner,~,~</v>
       </c>
       <c r="G54" s="3" t="str">
-        <f>CONCATENATE(A54,",",C54,",",B54,",",D54,",",E54)</f>
+        <f t="shared" si="3"/>
         <v>晩ご飯,dinner,ばんごはん,~,~</v>
       </c>
     </row>
@@ -14634,11 +14831,11 @@
         <v>7</v>
       </c>
       <c r="F55" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>味,あじ,taste,~,~</v>
       </c>
       <c r="G55" s="3" t="str">
-        <f>CONCATENATE(A55,",",C55,",",B55,",",D55,",",E55)</f>
+        <f t="shared" si="3"/>
         <v>味,taste,あじ,~,~</v>
       </c>
     </row>
@@ -14659,11 +14856,11 @@
         <v>7</v>
       </c>
       <c r="F56" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>意味,いみ,meaning,~,~</v>
       </c>
       <c r="G56" s="3" t="str">
-        <f>CONCATENATE(A56,",",C56,",",B56,",",D56,",",E56)</f>
+        <f t="shared" si="3"/>
         <v>意味,meaning,いみ,~,~</v>
       </c>
     </row>
@@ -14684,11 +14881,11 @@
         <v>7</v>
       </c>
       <c r="F57" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>代わる,かわる,take somebody’s place,~,~</v>
       </c>
       <c r="G57" s="3" t="str">
-        <f>CONCATENATE(A57,",",C57,",",B57,",",D57,",",E57)</f>
+        <f t="shared" si="3"/>
         <v>代わる,take somebody’s place,かわる,~,~</v>
       </c>
     </row>
@@ -14709,11 +14906,11 @@
         <v>7</v>
       </c>
       <c r="F58" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>代わりに,かわりに,instead,~,~</v>
       </c>
       <c r="G58" s="3" t="str">
-        <f>CONCATENATE(A58,",",C58,",",B58,",",D58,",",E58)</f>
+        <f t="shared" si="3"/>
         <v>代わりに,instead,かわりに,~,~</v>
       </c>
     </row>
@@ -14734,11 +14931,11 @@
         <v>7</v>
       </c>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>使う,つかう,to use,~,~</v>
       </c>
       <c r="G59" s="3" t="str">
-        <f>CONCATENATE(A59,",",C59,",",B59,",",D59,",",E59)</f>
+        <f t="shared" si="3"/>
         <v>使う,to use,つかう,~,~</v>
       </c>
     </row>
@@ -14759,11 +14956,11 @@
         <v>7</v>
       </c>
       <c r="F60" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>大使館,たいしかん,embassy,~,~</v>
       </c>
       <c r="G60" s="3" t="str">
-        <f>CONCATENATE(A60,",",C60,",",B60,",",D60,",",E60)</f>
+        <f t="shared" si="3"/>
         <v>大使館,embassy,たいしかん,~,~</v>
       </c>
     </row>
@@ -14784,11 +14981,11 @@
         <v>7</v>
       </c>
       <c r="F61" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>使用中,しようちゅう,be engaged on something,~,~</v>
       </c>
       <c r="G61" s="3" t="str">
-        <f>CONCATENATE(A61,",",C61,",",B61,",",D61,",",E61)</f>
+        <f t="shared" si="3"/>
         <v>使用中,be engaged on something,しようちゅう,~,~</v>
       </c>
     </row>
@@ -14809,11 +15006,11 @@
         <v>7</v>
       </c>
       <c r="F62" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>作る,つくる,to make,~,~</v>
       </c>
       <c r="G62" s="3" t="str">
-        <f>CONCATENATE(A62,",",C62,",",B62,",",D62,",",E62)</f>
+        <f t="shared" si="3"/>
         <v>作る,to make,つくる,~,~</v>
       </c>
     </row>
@@ -14834,11 +15031,11 @@
         <v>7</v>
       </c>
       <c r="F63" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>作文,さくぶん,essay,~,~</v>
       </c>
       <c r="G63" s="3" t="str">
-        <f>CONCATENATE(A63,",",C63,",",B63,",",D63,",",E63)</f>
+        <f t="shared" si="3"/>
         <v>作文,essay,さくぶん,~,~</v>
       </c>
     </row>
@@ -14859,11 +15056,11 @@
         <v>7</v>
       </c>
       <c r="F64" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>変化する,へんかする,to change,~,~</v>
       </c>
       <c r="G64" s="3" t="str">
-        <f>CONCATENATE(A64,",",C64,",",B64,",",D64,",",E64)</f>
+        <f t="shared" si="3"/>
         <v>変化する,to change,へんかする,~,~</v>
       </c>
     </row>
@@ -14884,11 +15081,11 @@
         <v>7</v>
       </c>
       <c r="F65" s="3" t="str">
-        <f t="shared" ref="F65:F71" si="2">CONCATENATE(A65,",",B65,",",C65,",",D65,",",E65)</f>
+        <f t="shared" ref="F65:F71" si="4">CONCATENATE(A65,",",B65,",",C65,",",D65,",",E65)</f>
         <v>信じる,しんじる,to believe,~,~</v>
       </c>
       <c r="G65" s="3" t="str">
-        <f>CONCATENATE(A65,",",C65,",",B65,",",D65,",",E65)</f>
+        <f t="shared" si="3"/>
         <v>信じる,to believe,しんじる,~,~</v>
       </c>
     </row>
@@ -14909,11 +15106,11 @@
         <v>7</v>
       </c>
       <c r="F66" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>信号,しんごう,signal,~,~</v>
       </c>
       <c r="G66" s="3" t="str">
-        <f>CONCATENATE(A66,",",C66,",",B66,",",D66,",",E66)</f>
+        <f t="shared" ref="G66:G71" si="5">CONCATENATE(A66,",",C66,",",B66,",",D66,",",E66)</f>
         <v>信号,signal,しんごう,~,~</v>
       </c>
     </row>
@@ -14934,11 +15131,11 @@
         <v>7</v>
       </c>
       <c r="F67" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>進む,すすむ,to proceed,~,~</v>
       </c>
       <c r="G67" s="3" t="str">
-        <f>CONCATENATE(A67,",",C67,",",B67,",",D67,",",E67)</f>
+        <f t="shared" si="5"/>
         <v>進む,to proceed,すすむ,~,~</v>
       </c>
     </row>
@@ -14959,11 +15156,11 @@
         <v>7</v>
       </c>
       <c r="F68" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>送る,おくる,to send,~,~</v>
       </c>
       <c r="G68" s="3" t="str">
-        <f>CONCATENATE(A68,",",C68,",",B68,",",D68,",",E68)</f>
+        <f t="shared" si="5"/>
         <v>送る,to send,おくる,~,~</v>
       </c>
     </row>
@@ -14984,11 +15181,11 @@
         <v>7</v>
       </c>
       <c r="F69" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>返す,かえす,to return,~,~</v>
       </c>
       <c r="G69" s="3" t="str">
-        <f>CONCATENATE(A69,",",C69,",",B69,",",D69,",",E69)</f>
+        <f t="shared" si="5"/>
         <v>返す,to return,かえす,~,~</v>
       </c>
     </row>
@@ -15009,11 +15206,11 @@
         <v>7</v>
       </c>
       <c r="F70" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>洗う,あらう,to wash,~,~</v>
       </c>
       <c r="G70" s="3" t="str">
-        <f>CONCATENATE(A70,",",C70,",",B70,",",D70,",",E70)</f>
+        <f t="shared" si="5"/>
         <v>洗う,to wash,あらう,~,~</v>
       </c>
     </row>
@@ -15034,20 +15231,20 @@
         <v>7</v>
       </c>
       <c r="F71" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>お手洗い,おてあらい,restroom,~,~</v>
       </c>
       <c r="G71" s="3" t="str">
-        <f>CONCATENATE(A71,",",C71,",",B71,",",D71,",",E71)</f>
+        <f t="shared" si="5"/>
         <v>お手洗い,restroom,おてあらい,~,~</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15116,11 +15313,11 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f t="shared" ref="F1:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <f t="shared" ref="F2:F32" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
         <v>場所,ばしょ,place,~,~</v>
       </c>
       <c r="G2" s="3" t="str">
-        <f>CONCATENATE(A2,",",C2,",",B2,",",D2,",",E2)</f>
+        <f t="shared" ref="G2:G33" si="1">CONCATENATE(A2,",",C2,",",B2,",",D2,",",E2)</f>
         <v>場所,place,ばしょ,~,~</v>
       </c>
     </row>
@@ -15145,7 +15342,7 @@
         <v>工場,こうじょう,factory,~,~</v>
       </c>
       <c r="G3" s="3" t="str">
-        <f>CONCATENATE(A3,",",C3,",",B3,",",D3,",",E3)</f>
+        <f t="shared" si="1"/>
         <v>工場,factory,こうじょう,~,~</v>
       </c>
     </row>
@@ -15170,7 +15367,7 @@
         <v>建てる,たてる,to build,~,~</v>
       </c>
       <c r="G4" s="3" t="str">
-        <f>CONCATENATE(A4,",",C4,",",B4,",",D4,",",E4)</f>
+        <f t="shared" si="1"/>
         <v>建てる,to build,たてる,~,~</v>
       </c>
     </row>
@@ -15195,7 +15392,7 @@
         <v>建物,たてもの,building,~,~</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>CONCATENATE(A5,",",C5,",",B5,",",D5,",",E5)</f>
+        <f t="shared" si="1"/>
         <v>建物,building,たてもの,~,~</v>
       </c>
     </row>
@@ -15220,7 +15417,7 @@
         <v>物,もの,things,~,~</v>
       </c>
       <c r="G6" s="3" t="str">
-        <f>CONCATENATE(A6,",",C6,",",B6,",",D6,",",E6)</f>
+        <f t="shared" si="1"/>
         <v>物,things,もの,~,~</v>
       </c>
     </row>
@@ -15245,7 +15442,7 @@
         <v>買い物,かいもの,shopping,~,~</v>
       </c>
       <c r="G7" s="3" t="str">
-        <f>CONCATENATE(A7,",",C7,",",B7,",",D7,",",E7)</f>
+        <f t="shared" si="1"/>
         <v>買い物,shopping,かいもの,~,~</v>
       </c>
     </row>
@@ -15270,7 +15467,7 @@
         <v>動物,どうぶつ,animal,~,~</v>
       </c>
       <c r="G8" s="3" t="str">
-        <f>CONCATENATE(A8,",",C8,",",B8,",",D8,",",E8)</f>
+        <f t="shared" si="1"/>
         <v>動物,animal,どうぶつ,~,~</v>
       </c>
     </row>
@@ -15295,7 +15492,7 @@
         <v>病院,びょういん,hospital,~,~</v>
       </c>
       <c r="G9" s="3" t="str">
-        <f>CONCATENATE(A9,",",C9,",",B9,",",D9,",",E9)</f>
+        <f t="shared" si="1"/>
         <v>病院,hospital,びょういん,~,~</v>
       </c>
     </row>
@@ -15320,7 +15517,7 @@
         <v>入院する,にゅういんする,to be hospitalized,~,~</v>
       </c>
       <c r="G10" s="3" t="str">
-        <f>CONCATENATE(A10,",",C10,",",B10,",",D10,",",E10)</f>
+        <f t="shared" si="1"/>
         <v>入院する,to be hospitalized,にゅういんする,~,~</v>
       </c>
     </row>
@@ -15345,7 +15542,7 @@
         <v>大学院,だいがくいん,graduate school,~,~</v>
       </c>
       <c r="G11" s="3" t="str">
-        <f>CONCATENATE(A11,",",C11,",",B11,",",D11,",",E11)</f>
+        <f t="shared" si="1"/>
         <v>大学院,graduate school,だいがくいん,~,~</v>
       </c>
     </row>
@@ -15370,7 +15567,7 @@
         <v>映画館,えいがかん,movie theater,~,~</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f>CONCATENATE(A12,",",C12,",",B12,",",D12,",",E12)</f>
+        <f t="shared" si="1"/>
         <v>映画館,movie theater,えいがかん,~,~</v>
       </c>
     </row>
@@ -15395,7 +15592,7 @@
         <v>大使館,たいしかん,embassy,~,~</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f>CONCATENATE(A13,",",C13,",",B13,",",D13,",",E13)</f>
+        <f t="shared" si="1"/>
         <v>大使館,embassy,たいしかん,~,~</v>
       </c>
     </row>
@@ -15420,7 +15617,7 @@
         <v>食堂,しょくどう,dining room,~,~</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>CONCATENATE(A14,",",C14,",",B14,",",D14,",",E14)</f>
+        <f t="shared" si="1"/>
         <v>食堂,dining room,しょくどう,~,~</v>
       </c>
     </row>
@@ -15445,7 +15642,7 @@
         <v>教室,きょうしつ,classroom,~,~</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f>CONCATENATE(A15,",",C15,",",B15,",",D15,",",E15)</f>
+        <f t="shared" si="1"/>
         <v>教室,classroom,きょうしつ,~,~</v>
       </c>
     </row>
@@ -15470,7 +15667,7 @@
         <v>工事,こうじ,construction,~,~</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f>CONCATENATE(A16,",",C16,",",B16,",",D16,",",E16)</f>
+        <f t="shared" si="1"/>
         <v>工事,construction,こうじ,~,~</v>
       </c>
     </row>
@@ -15495,7 +15692,7 @@
         <v>工業,こうぎょう,manufacturing,~,~</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f>CONCATENATE(A17,",",C17,",",B17,",",D17,",",E17)</f>
+        <f t="shared" si="1"/>
         <v>工業,manufacturing,こうぎょう,~,~</v>
       </c>
     </row>
@@ -15520,7 +15717,7 @@
         <v>図,ず,figure,~,~</v>
       </c>
       <c r="G18" s="3" t="str">
-        <f>CONCATENATE(A18,",",C18,",",B18,",",D18,",",E18)</f>
+        <f t="shared" si="1"/>
         <v>図,figure,ず,~,~</v>
       </c>
     </row>
@@ -15545,7 +15742,7 @@
         <v>地図,ちず,map,~,~</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f>CONCATENATE(A19,",",C19,",",B19,",",D19,",",E19)</f>
+        <f t="shared" si="1"/>
         <v>地図,map,ちず,~,~</v>
       </c>
     </row>
@@ -15570,7 +15767,7 @@
         <v>図書館,としょかん,library,~,~</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f>CONCATENATE(A20,",",C20,",",B20,",",D20,",",E20)</f>
+        <f t="shared" si="1"/>
         <v>図書館,library,としょかん,~,~</v>
       </c>
     </row>
@@ -15595,7 +15792,7 @@
         <v>信号,しんごう,signal,~,~</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f>CONCATENATE(A21,",",C21,",",B21,",",D21,",",E21)</f>
+        <f t="shared" si="1"/>
         <v>信号,signal,しんごう,~,~</v>
       </c>
     </row>
@@ -15620,7 +15817,7 @@
         <v>交通,こうつう,traffic,~,~</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f>CONCATENATE(A22,",",C22,",",B22,",",D22,",",E22)</f>
+        <f t="shared" si="1"/>
         <v>交通,traffic,こうつう,~,~</v>
       </c>
     </row>
@@ -15645,7 +15842,7 @@
         <v>通る,とおる,to go through,~,~</v>
       </c>
       <c r="G23" s="3" t="str">
-        <f>CONCATENATE(A23,",",C23,",",B23,",",D23,",",E23)</f>
+        <f t="shared" si="1"/>
         <v>通る,to go through,とおる,~,~</v>
       </c>
     </row>
@@ -15670,7 +15867,7 @@
         <v>通う,かよう,to commute,~,~</v>
       </c>
       <c r="G24" s="3" t="str">
-        <f>CONCATENATE(A24,",",C24,",",B24,",",D24,",",E24)</f>
+        <f t="shared" si="1"/>
         <v>通う,to commute,かよう,~,~</v>
       </c>
     </row>
@@ -15695,7 +15892,7 @@
         <v>通学,つうがく,commute to school,~,~</v>
       </c>
       <c r="G25" s="3" t="str">
-        <f>CONCATENATE(A25,",",C25,",",B25,",",D25,",",E25)</f>
+        <f t="shared" si="1"/>
         <v>通学,commute to school,つうがく,~,~</v>
       </c>
     </row>
@@ -15720,7 +15917,7 @@
         <v>大通り,おおどおり,main street,~,~</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>CONCATENATE(A26,",",C26,",",B26,",",D26,",",E26)</f>
+        <f t="shared" si="1"/>
         <v>大通り,main street,おおどおり,~,~</v>
       </c>
     </row>
@@ -15745,7 +15942,7 @@
         <v>動く,うごく,to move,~,~</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f>CONCATENATE(A27,",",C27,",",B27,",",D27,",",E27)</f>
+        <f t="shared" si="1"/>
         <v>動く,to move,うごく,~,~</v>
       </c>
     </row>
@@ -15770,7 +15967,7 @@
         <v>運動,うんどう,exercise,~,~</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f>CONCATENATE(A28,",",C28,",",B28,",",D28,",",E28)</f>
+        <f t="shared" si="1"/>
         <v>運動,exercise,うんどう,~,~</v>
       </c>
     </row>
@@ -15795,7 +15992,7 @@
         <v>自動車,じどうしゃ,car,~,~</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f>CONCATENATE(A29,",",C29,",",B29,",",D29,",",E29)</f>
+        <f t="shared" si="1"/>
         <v>自動車,car,じどうしゃ,~,~</v>
       </c>
     </row>
@@ -15820,7 +16017,7 @@
         <v>乗る,のる,to get on,~,~</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f>CONCATENATE(A30,",",C30,",",B30,",",D30,",",E30)</f>
+        <f t="shared" si="1"/>
         <v>乗る,to get on,のる,~,~</v>
       </c>
     </row>
@@ -15845,7 +16042,7 @@
         <v>乗り場,のりば,transport stop/stand,~,~</v>
       </c>
       <c r="G31" s="3" t="str">
-        <f>CONCATENATE(A31,",",C31,",",B31,",",D31,",",E31)</f>
+        <f t="shared" si="1"/>
         <v>乗り場,transport stop/stand,のりば,~,~</v>
       </c>
     </row>
@@ -15870,7 +16067,7 @@
         <v>降りる,おりる,to get off,~,~</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f>CONCATENATE(A32,",",C32,",",B32,",",D32,",",E32)</f>
+        <f t="shared" si="1"/>
         <v>降りる,to get off,おりる,~,~</v>
       </c>
     </row>
@@ -15891,11 +16088,11 @@
         <v>7</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f t="shared" ref="F33:F58" si="1">CONCATENATE(A33,",",B33,",",C33,",",D33,",",E33)</f>
+        <f t="shared" ref="F33:F58" si="2">CONCATENATE(A33,",",B33,",",C33,",",D33,",",E33)</f>
         <v>降る,ふる,to rain,~,~</v>
       </c>
       <c r="G33" s="3" t="str">
-        <f>CONCATENATE(A33,",",C33,",",B33,",",D33,",",E33)</f>
+        <f t="shared" si="1"/>
         <v>降る,to rain,ふる,~,~</v>
       </c>
     </row>
@@ -15916,11 +16113,11 @@
         <v>7</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>運ぶ,はこぶ,to transport,~,~</v>
       </c>
       <c r="G34" s="3" t="str">
-        <f>CONCATENATE(A34,",",C34,",",B34,",",D34,",",E34)</f>
+        <f t="shared" ref="G34:G58" si="3">CONCATENATE(A34,",",C34,",",B34,",",D34,",",E34)</f>
         <v>運ぶ,to transport,はこぶ,~,~</v>
       </c>
     </row>
@@ -15941,11 +16138,11 @@
         <v>7</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>運転する,うんてんする,to drive,~,~</v>
       </c>
       <c r="G35" s="3" t="str">
-        <f>CONCATENATE(A35,",",C35,",",B35,",",D35,",",E35)</f>
+        <f t="shared" si="3"/>
         <v>運転する,to drive,うんてんする,~,~</v>
       </c>
     </row>
@@ -15966,11 +16163,11 @@
         <v>7</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>自転車,じてんしゃ,bicycle,~,~</v>
       </c>
       <c r="G36" s="3" t="str">
-        <f>CONCATENATE(A36,",",C36,",",B36,",",D36,",",E36)</f>
+        <f t="shared" si="3"/>
         <v>自転車,bicycle,じてんしゃ,~,~</v>
       </c>
     </row>
@@ -15991,11 +16188,11 @@
         <v>7</v>
       </c>
       <c r="F37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>帰る,かえる,to return,~,~</v>
       </c>
       <c r="G37" s="3" t="str">
-        <f>CONCATENATE(A37,",",C37,",",B37,",",D37,",",E37)</f>
+        <f t="shared" si="3"/>
         <v>帰る,to return,かえる,~,~</v>
       </c>
     </row>
@@ -16016,11 +16213,11 @@
         <v>7</v>
       </c>
       <c r="F38" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>帰国する,きこくする,to return one’s country,~,~</v>
       </c>
       <c r="G38" s="3" t="str">
-        <f>CONCATENATE(A38,",",C38,",",B38,",",D38,",",E38)</f>
+        <f t="shared" si="3"/>
         <v>帰国する,to return one’s country,きこくする,~,~</v>
       </c>
     </row>
@@ -16041,11 +16238,11 @@
         <v>7</v>
       </c>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>お帰りなさい,おかえりなさい,welcome home,~,~</v>
       </c>
       <c r="G39" s="3" t="str">
-        <f>CONCATENATE(A39,",",C39,",",B39,",",D39,",",E39)</f>
+        <f t="shared" si="3"/>
         <v>お帰りなさい,welcome home,おかえりなさい,~,~</v>
       </c>
     </row>
@@ -16066,11 +16263,11 @@
         <v>7</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>出発する,しゅっぱつする,to leave,~,~</v>
       </c>
       <c r="G40" s="3" t="str">
-        <f>CONCATENATE(A40,",",C40,",",B40,",",D40,",",E40)</f>
+        <f t="shared" si="3"/>
         <v>出発する,to leave,しゅっぱつする,~,~</v>
       </c>
     </row>
@@ -16091,11 +16288,11 @@
         <v>7</v>
       </c>
       <c r="F41" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>着る,きる,to put on clothes,~,~</v>
       </c>
       <c r="G41" s="3" t="str">
-        <f>CONCATENATE(A41,",",C41,",",B41,",",D41,",",E41)</f>
+        <f t="shared" si="3"/>
         <v>着る,to put on clothes,きる,~,~</v>
       </c>
     </row>
@@ -16116,11 +16313,11 @@
         <v>7</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>着く,つく,to arrive,~,~</v>
       </c>
       <c r="G42" s="3" t="str">
-        <f>CONCATENATE(A42,",",C42,",",B42,",",D42,",",E42)</f>
+        <f t="shared" si="3"/>
         <v>着く,to arrive,つく,~,~</v>
       </c>
     </row>
@@ -16141,11 +16338,11 @@
         <v>7</v>
       </c>
       <c r="F43" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>着物,きもの,Kimono,~,~</v>
       </c>
       <c r="G43" s="3" t="str">
-        <f>CONCATENATE(A43,",",C43,",",B43,",",D43,",",E43)</f>
+        <f t="shared" si="3"/>
         <v>着物,Kimono,きもの,~,~</v>
       </c>
     </row>
@@ -16166,11 +16363,11 @@
         <v>7</v>
       </c>
       <c r="F44" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>漢字,かんじ,Kanji,~,~</v>
       </c>
       <c r="G44" s="3" t="str">
-        <f>CONCATENATE(A44,",",C44,",",B44,",",D44,",",E44)</f>
+        <f t="shared" si="3"/>
         <v>漢字,Kanji,かんじ,~,~</v>
       </c>
     </row>
@@ -16191,11 +16388,11 @@
         <v>7</v>
       </c>
       <c r="F45" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>字,じ,letter,~,~</v>
       </c>
       <c r="G45" s="3" t="str">
-        <f>CONCATENATE(A45,",",C45,",",B45,",",D45,",",E45)</f>
+        <f t="shared" si="3"/>
         <v>字,letter,じ,~,~</v>
       </c>
     </row>
@@ -16216,11 +16413,11 @@
         <v>7</v>
       </c>
       <c r="F46" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>文字,もじ,character,~,~</v>
       </c>
       <c r="G46" s="3" t="str">
-        <f>CONCATENATE(A46,",",C46,",",B46,",",D46,",",E46)</f>
+        <f t="shared" si="3"/>
         <v>文字,character,もじ,~,~</v>
       </c>
     </row>
@@ -16241,11 +16438,11 @@
         <v>7</v>
       </c>
       <c r="F47" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>文,ぶん,sentence,~,~</v>
       </c>
       <c r="G47" s="3" t="str">
-        <f>CONCATENATE(A47,",",C47,",",B47,",",D47,",",E47)</f>
+        <f t="shared" si="3"/>
         <v>文,sentence,ぶん,~,~</v>
       </c>
     </row>
@@ -16266,11 +16463,11 @@
         <v>7</v>
       </c>
       <c r="F48" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>文学,ぶんがく,literature,~,~</v>
       </c>
       <c r="G48" s="3" t="str">
-        <f>CONCATENATE(A48,",",C48,",",B48,",",D48,",",E48)</f>
+        <f t="shared" si="3"/>
         <v>文学,literature,ぶんがく,~,~</v>
       </c>
     </row>
@@ -16291,11 +16488,11 @@
         <v>7</v>
       </c>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>教える,おしえる,to teach,~,~</v>
       </c>
       <c r="G49" s="3" t="str">
-        <f>CONCATENATE(A49,",",C49,",",B49,",",D49,",",E49)</f>
+        <f t="shared" si="3"/>
         <v>教える,to teach,おしえる,~,~</v>
       </c>
     </row>
@@ -16316,11 +16513,11 @@
         <v>7</v>
       </c>
       <c r="F50" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>教室,きょうしつ,classroom,~,~</v>
       </c>
       <c r="G50" s="3" t="str">
-        <f>CONCATENATE(A50,",",C50,",",B50,",",D50,",",E50)</f>
+        <f t="shared" si="3"/>
         <v>教室,classroom,きょうしつ,~,~</v>
       </c>
     </row>
@@ -16341,11 +16538,11 @@
         <v>7</v>
       </c>
       <c r="F51" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>教科書,きょうかしょ,text book,~,~</v>
       </c>
       <c r="G51" s="3" t="str">
-        <f>CONCATENATE(A51,",",C51,",",B51,",",D51,",",E51)</f>
+        <f t="shared" si="3"/>
         <v>教科書,text book,きょうかしょ,~,~</v>
       </c>
     </row>
@@ -16366,11 +16563,11 @@
         <v>7</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>勉強する,べんきょうする,to study,~,~</v>
       </c>
       <c r="G52" s="3" t="str">
-        <f>CONCATENATE(A52,",",C52,",",B52,",",D52,",",E52)</f>
+        <f t="shared" si="3"/>
         <v>勉強する,to study,べんきょうする,~,~</v>
       </c>
     </row>
@@ -16391,11 +16588,11 @@
         <v>7</v>
       </c>
       <c r="F53" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>習う,ならう,to learn,~,~</v>
       </c>
       <c r="G53" s="3" t="str">
-        <f>CONCATENATE(A53,",",C53,",",B53,",",D53,",",E53)</f>
+        <f t="shared" si="3"/>
         <v>習う,to learn,ならう,~,~</v>
       </c>
     </row>
@@ -16416,11 +16613,11 @@
         <v>7</v>
       </c>
       <c r="F54" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>英語,えいご,English,~,~</v>
       </c>
       <c r="G54" s="3" t="str">
-        <f>CONCATENATE(A54,",",C54,",",B54,",",D54,",",E54)</f>
+        <f t="shared" si="3"/>
         <v>英語,English,えいご,~,~</v>
       </c>
     </row>
@@ -16441,11 +16638,11 @@
         <v>7</v>
       </c>
       <c r="F55" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>考える,かんがえる,to think,~,~</v>
       </c>
       <c r="G55" s="3" t="str">
-        <f>CONCATENATE(A55,",",C55,",",B55,",",D55,",",E55)</f>
+        <f t="shared" si="3"/>
         <v>考える,to think,かんがえる,~,~</v>
       </c>
     </row>
@@ -16466,11 +16663,11 @@
         <v>7</v>
       </c>
       <c r="F56" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>研究する,けんきゅうする,do research,~,~</v>
       </c>
       <c r="G56" s="3" t="str">
-        <f>CONCATENATE(A56,",",C56,",",B56,",",D56,",",E56)</f>
+        <f t="shared" si="3"/>
         <v>研究する,do research,けんきゅうする,~,~</v>
       </c>
     </row>
@@ -16491,11 +16688,11 @@
         <v>7</v>
       </c>
       <c r="F57" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>研究者,けんきゅうしゃ,researcher,~,~</v>
       </c>
       <c r="G57" s="3" t="str">
-        <f>CONCATENATE(A57,",",C57,",",B57,",",D57,",",E57)</f>
+        <f t="shared" si="3"/>
         <v>研究者,researcher,けんきゅうしゃ,~,~</v>
       </c>
     </row>
@@ -16516,11 +16713,11 @@
         <v>7</v>
       </c>
       <c r="F58" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>研究室,けんきゅうしつ,laboratory,~,~</v>
       </c>
       <c r="G58" s="3" t="str">
-        <f>CONCATENATE(A58,",",C58,",",B58,",",D58,",",E58)</f>
+        <f t="shared" si="3"/>
         <v>研究室,laboratory,けんきゅうしつ,~,~</v>
       </c>
     </row>
@@ -16532,7 +16729,7 @@
     <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16543,9 +16740,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16601,7 +16798,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f t="shared" ref="F1:F39" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <f t="shared" ref="F2:F39" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
         <v>問,とい,question,~,~</v>
       </c>
       <c r="G2" s="3" t="str">
@@ -17608,12 +17805,983 @@
     </row>
     <row r="58" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D58" s="7"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:C1">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="48" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <f>CONCATENATE(A1,",",B1,",",C1,",",D1,",",E1)</f>
+        <v>漢字,答え,ヒント,例（日本語）,例（英語）</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <f>CONCATENATE(A1,",",B1,",",C1,",",D1,",",E1)</f>
+        <v>漢字,答え,ヒント,例（日本語）,例（英語）</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f t="shared" ref="F2" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <v>駐,ちゅう;cyuu;chuu,stop-over;reside in;resident,~,~</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f t="shared" ref="G2" si="1">CONCATENATE(A2,",",C2,",",B2,",",D2,",",E2)</f>
+        <v>駐,stop-over;reside in;resident,ちゅう;cyuu;chuu,~,~</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F38" si="2">CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3)</f>
+        <v>駐車,ちゅうしゃ;cyuusya;chuusya;cyuusha;chuusha,park;parking,~,~</v>
+      </c>
+      <c r="G3" s="3" t="str">
+        <f t="shared" ref="G3:G38" si="3">CONCATENATE(A3,",",C3,",",B3,",",D3,",",E3)</f>
+        <v>駐車,park;parking,ちゅうしゃ;cyuusya;chuusya;cyuusha;chuusha,~,~</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>駐車場,ちゅうしゃじょう;cyuusyajyou;chuusyajyou;cyuushajyou;chuushajyou,parking lot,~,~</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>駐車場,parking lot,ちゅうしゃじょう;cyuusyajyou;chuusyajyou;cyuushajyou;chuushajyou,~,~</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>無,む;ない;mu;nai,not existing; none,~,~</v>
+      </c>
+      <c r="G5" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>無,not existing; none,む;ない;mu;nai,~,~</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" ref="F6" si="4">CONCATENATE(A6,",",B6,",",C6,",",D6,",",E6)</f>
+        <v>無休,むきゅう;mukyuu,work without a holiday;work without a holiday,~,~</v>
+      </c>
+      <c r="G6" s="3" t="str">
+        <f t="shared" ref="G6" si="5">CONCATENATE(A6,",",C6,",",B6,",",D6,",",E6)</f>
+        <v>無休,work without a holiday;work without a holiday,むきゅう;mukyuu,~,~</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>無理(な),むり;むりな;muri;murina,unreasonable;impossible,~,~</v>
+      </c>
+      <c r="G7" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>無理(な),unreasonable;impossible,むり;むりな;muri;murina,~,~</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>無料,むりょう;muryou,free;free of charge,~,~</v>
+      </c>
+      <c r="G8" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>無料,free;free of charge,むりょう;muryou,~,~</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>無い,ない;nai,does not exist;do not have;gone,~,~</v>
+      </c>
+      <c r="G9" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>無い,does not exist;do not have;gone,ない;nai,~,~</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>満,まん;man,being full;full,~,~</v>
+      </c>
+      <c r="G10" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>満,being full;full,まん;man,~,~</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>満車,まんしゃ;mansya;mansha,full of cars;full (of cars);full(of cars),~,~</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>満車,full of cars;full (of cars);full(of cars),まんしゃ;mansya;mansha,~,~</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>不満(な),ふまん;ふまんな;fuman;fumanna,dissatisfaction;dissatisfied,~,~</v>
+      </c>
+      <c r="G12" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>不満(な),dissatisfaction;dissatisfied,ふまん;ふまんな;fuman;fumanna,~,~</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>満員,まんいん;manin;manin,full of people;full (of people);full(of people),~,~</v>
+      </c>
+      <c r="G13" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>満員,full of people;full (of people);full(of people),まんいん;manin;manin,~,~</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>向,こう;むこう;むかう;むき;kou;mukou;mukau;muki,facing;toward;beyond,~,~</v>
+      </c>
+      <c r="G14" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>向,facing;toward;beyond,こう;むこう;むかう;むき;kou;mukou;mukau;muki,~,~</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f>CONCATENATE(A15,",",B15,",",C15,",",D15,",",E15)</f>
+        <v>方向,ほうこう;houkou,direction,~,~</v>
+      </c>
+      <c r="G15" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>方向,direction,ほうこう;houkou,~,~</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>向かう,向かう;mukau,go forward,~,~</v>
+      </c>
+      <c r="G16" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>向かう,go forward,向かう;mukau,~,~</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>向こう,むこう;mukou,over there;beyond,~,~</v>
+      </c>
+      <c r="G17" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>向こう,over there;beyond,むこう;mukou,~,~</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>○○向き,むき;muki,suitable for,~,~</v>
+      </c>
+      <c r="G18" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>○○向き,suitable for,むき;muki,~,~</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>禁,きん;kin,ban;prohibition,~,~</v>
+      </c>
+      <c r="G19" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>禁,ban;prohibition,きん;kin,~,~</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>禁止,きんし;kinshi,ban;prohibition,~,~</v>
+      </c>
+      <c r="G20" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>禁止,ban;prohibition,きんし;kinshi,~,~</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>関,かん;せき;kan;seki;,barrier;gate;connection;related,~,~</v>
+      </c>
+      <c r="G21" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>関,barrier;gate;connection;related,かん;せき;kan;seki;,~,~</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>関心,かんしん;kanshin,interest,~,~</v>
+      </c>
+      <c r="G22" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>関心,interest,かんしん;kanshin,~,~</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>関する,かんする;kansuru,related,~,~</v>
+      </c>
+      <c r="G23" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>関する,related,かんする;kansuru,~,~</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>関係,かんけい;kankei,relation;connection,~,~</v>
+      </c>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>関係,relation;connection,かんけい;kankei,~,~</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>係,かかり;kakari,person in charge,~,~</v>
+      </c>
+      <c r="G25" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>係,person in charge,かかり;kakari,~,~</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>断,だん;dan,decision;judgement;resolution,~,~</v>
+      </c>
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>断,decision;judgement;resolution,だん;dan,~,~</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>1482</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>無断,むだん;mudan,without permission,~,~</v>
+      </c>
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>無断,without permission,むだん;mudan,~,~</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>断る,ことわる;kotowaru,refuse,~,~</v>
+      </c>
+      <c r="G28" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>断る,refuse,ことわる;kotowaru,~,~</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>断水,だんすい;dansui,suspension of water supply,~,~</v>
+      </c>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>断水,suspension of water supply,だんすい;dansui,~,~</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G31" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G35" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G36" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>,,,~,~</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>,,,~,~</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="4:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="4:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="D57" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>